<commit_message>
Feature Envy y Inappropriate Intimacy
</commit_message>
<xml_diff>
--- a/RefactoringExelMoya.xlsx
+++ b/RefactoringExelMoya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel Moya\Documents\Luis Angel\Espol\Septimo semestre\Diseño de Software\Refactoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A7C657FC-7AEF-4318-8444-4D83AA360EC1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37E11F89-07B6-45F4-BEAC-23DE8C6152DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{122B9872-7810-4D28-B032-B99758B7FF82}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Long Method</t>
   </si>
@@ -42,12 +42,6 @@
     <t>TECNICA DE REFACTORIZACIÓN</t>
   </si>
   <si>
-    <t>Español</t>
-  </si>
-  <si>
-    <t>Ingles</t>
-  </si>
-  <si>
     <t>BIBLIOGRAFIA</t>
   </si>
   <si>
@@ -171,24 +165,6 @@
     <t>Codigo Duplicado</t>
   </si>
   <si>
-    <t>Columna1</t>
-  </si>
-  <si>
-    <t>Columna2</t>
-  </si>
-  <si>
-    <t>Columna3</t>
-  </si>
-  <si>
-    <t>Columna4</t>
-  </si>
-  <si>
-    <t>Columna5</t>
-  </si>
-  <si>
-    <t>Columna6</t>
-  </si>
-  <si>
     <t>Clase de Datos</t>
   </si>
   <si>
@@ -196,6 +172,33 @@
   </si>
   <si>
     <t>- Se debera encapsular los campos de la clase haciendo privado a los atributos y agregando metodos de acceso a dichos atributos.                                                                        - Dependiendo de las funcionalidades de cada clase se puede aplicar Move Method y Extract Method para establecer la funcionalidad de cada clase.                                                                                       -Si se desea que los atributos no cambien se debe de eliminar los metodos de acceso y estos unicamente cambiaran al ser instanciados.</t>
+  </si>
+  <si>
+    <t>Intimidad inapropiada</t>
+  </si>
+  <si>
+    <t>Ocurre cuando un metodo utiliza los datos de otro metodo mas que los propios.</t>
+  </si>
+  <si>
+    <t>- EL metodo de otra clase que es mayormente utilizado se tendra que mover al nuestra clase.                                - Cuando se utiliza funciones de otras clases, se tendrá que tomar la clase la cual contiene el metodo mas utilizado por nuestro clase y agregar el resto de funcionalidades a dicha clase haciendo extraccion de metodo.</t>
+  </si>
+  <si>
+    <t>Envidia de caracteristicas</t>
+  </si>
+  <si>
+    <t>https://www.slideshare.net/MrinalBhattacaharya/code-smells-52370759</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Ocurre cuando una clase utiliza metodos o atibutos internos de otra clase.</t>
+  </si>
+  <si>
+    <t>- El metodo deberia implementar dicho metodo para que sea propio. (Move Method)                                                           - El metodo utilizado por ambas clases se deberia implementar en una clase externa (Extract Class).                                  - Si ambas clases comparten metodos lo mas recomendable es crear una clase padre con dicho metodo.</t>
+  </si>
+  <si>
+    <t>http://siloracle.blogspot.com/2014/11/code-smells-inappropriate-intimacy-with.html</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -312,46 +315,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -387,18 +355,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -580,15 +536,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4A655B1-D14C-401F-AEEA-E4629DD8A28D}" name="Tabla1" displayName="Tabla1" ref="B2:G16" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="B2:G16" xr:uid="{A353535F-3A55-4AAE-B5D2-9EC2A734294A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4A655B1-D14C-401F-AEEA-E4629DD8A28D}" name="Tabla1" displayName="Tabla1" ref="B4:G16" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B4:G16" xr:uid="{A353535F-3A55-4AAE-B5D2-9EC2A734294A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A108CF69-FC23-45B6-8481-40546EB6AE1A}" name="Columna1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{79BA20ED-2427-44B4-B538-FF27A975A335}" name="Columna2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D0BACB97-D08D-4087-B1EB-6733B10D343A}" name="Columna3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{F86C6687-E4AC-4264-9907-62EB9FF7B20F}" name="Columna4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{231770CD-AE49-4C5E-9798-F44E2719F679}" name="Columna5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{949C35AE-7AAD-4CA6-82FB-EA38882547D7}" name="Columna6" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A108CF69-FC23-45B6-8481-40546EB6AE1A}" name="NOMBRE" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{79BA20ED-2427-44B4-B538-FF27A975A335}" name="Name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D0BACB97-D08D-4087-B1EB-6733B10D343A}" name="DESCRIPCIÓN" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F86C6687-E4AC-4264-9907-62EB9FF7B20F}" name="TECNICA DE REFACTORIZACIÓN" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{231770CD-AE49-4C5E-9798-F44E2719F679}" name="ENLACE GIT" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{949C35AE-7AAD-4CA6-82FB-EA38882547D7}" name="BIBLIOGRAFIA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -891,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6001782D-0BB8-4B33-B08D-82D74B02D928}">
-  <dimension ref="B1:I16"/>
+  <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,66 +863,38 @@
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="C4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:9" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="F4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -978,205 +906,221 @@
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:9" ht="165" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="2:9" ht="150" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="2:9" ht="150" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="2:9" ht="150" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:9" ht="199.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
+    <row r="14" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="16"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>